<commit_message>
-Updated project activity spreadsheet
</commit_message>
<xml_diff>
--- a/ProjectManagement/ActivitiesTracker.xlsx
+++ b/ProjectManagement/ActivitiesTracker.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>Activity</t>
   </si>
@@ -41,15 +41,9 @@
     <t>Create Template Liquid</t>
   </si>
   <si>
-    <t>Create  Snippet Liquid</t>
-  </si>
-  <si>
     <t>Create Image Slider Liquid</t>
   </si>
   <si>
-    <t>Create Navigation Slider Liquid</t>
-  </si>
-  <si>
     <t>Responsibility</t>
   </si>
   <si>
@@ -114,12 +108,45 @@
   </si>
   <si>
     <t>Create Rich Text Liquid</t>
+  </si>
+  <si>
+    <t>Enumerate Snippet Types</t>
+  </si>
+  <si>
+    <t>Create  Snippet Liquids</t>
+  </si>
+  <si>
+    <t>Expected Work Effort (Hrs)</t>
+  </si>
+  <si>
+    <t>Research Testing Framework</t>
+  </si>
+  <si>
+    <t>Implement Testing Framework</t>
+  </si>
+  <si>
+    <t>Create Navigation Liquid</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Bobby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,149 +470,411 @@
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>37.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="F23">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F26">
+        <v>37.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>17</v>
+      <c r="G28" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -592,5 +882,6 @@
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>